<commit_message>
1.8 excel interfaces done, second one fought a little
</commit_message>
<xml_diff>
--- a/public/formatos/Formato Data Epidemiológica/Formato Data Epidemiológica 2025.xlsx
+++ b/public/formatos/Formato Data Epidemiológica/Formato Data Epidemiológica 2025.xlsx
@@ -1,27 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="261"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="261" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="2025" sheetId="1" r:id="rId1"/>
+    <sheet name="2025" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2025'!$A$6:$AJ$62</definedName>
-  </definedNames>
-  <calcPr calcId="125725"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
   <si>
     <t>TIPO DE EVENTO</t>
   </si>
   <si>
+    <t>CLASIFICACION ANTERIOR</t>
+  </si>
+  <si>
+    <t>FORMATO DE DATA EPIDEMIOLOGICA</t>
+  </si>
+  <si>
+    <t>Plagas comunes</t>
+  </si>
+  <si>
+    <t>Presuntivo</t>
+  </si>
+  <si>
+    <t>Plaga cuarentenaria</t>
+  </si>
+  <si>
+    <t>Sin Novedad</t>
+  </si>
+  <si>
     <t>REGISTRO DE NOTIFICACION</t>
   </si>
   <si>
@@ -55,6 +71,9 @@
     <t>SECTOR</t>
   </si>
   <si>
+    <t>LUGAR O SITIO DONDE SE REALIZA LA INSPECCION (Predio, Unidad de Producción, Vehículo de Carga, Patios Productivos, Vivero, Casas de Cultivos, etc)</t>
+  </si>
+  <si>
     <t>DIRECCION DE LA UNIDAD QUE SE INSPECCIONO</t>
   </si>
   <si>
@@ -124,329 +143,194 @@
     <t>RESPONSABLE DE LA TRANSCRIPCION</t>
   </si>
   <si>
-    <t>Sin Novedad</t>
-  </si>
-  <si>
-    <t>LUGAR O SITIO DONDE SE REALIZA LA INSPECCION (Predio, Unidad de Producción, Vehículo de Carga, Patios Productivos, Vivero, Casas de Cultivos, etc)</t>
-  </si>
-  <si>
-    <t>CLASIFICACION ANTERIOR</t>
-  </si>
-  <si>
-    <t>Plagas comunes</t>
-  </si>
-  <si>
-    <t>Presuntivo</t>
-  </si>
-  <si>
-    <t>Plaga cuarentenaria</t>
-  </si>
-  <si>
-    <t>FORMATO DE DATA EPIDEMIOLOGICA</t>
-  </si>
-  <si>
     <t>algo</t>
   </si>
   <si>
     <t>Unidad de Produccion</t>
+  </si>
+  <si>
+    <t>asdagad</t>
+  </si>
+  <si>
+    <t>hola</t>
+  </si>
+  <si>
+    <t>11/04/2025</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>vehiculo</t>
+  </si>
+  <si>
+    <t>aswertfgyjh</t>
+  </si>
+  <si>
+    <t>Yuca</t>
+  </si>
+  <si>
+    <t>saludos</t>
+  </si>
+  <si>
+    <t>unidades</t>
+  </si>
+  <si>
+    <t>parte</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>nombre5</t>
+  </si>
+  <si>
+    <t>J-50000005-5</t>
+  </si>
+  <si>
+    <t>punto</t>
+  </si>
+  <si>
+    <t>lab</t>
+  </si>
+  <si>
+    <t>24/04/2025</t>
+  </si>
+  <si>
+    <t>Se ve raro</t>
+  </si>
+  <si>
+    <t>nombre4</t>
+  </si>
+  <si>
+    <t>Responsable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="169" formatCode="* #,##0.00&quot; € &quot;;\-* #,##0.00&quot; € &quot;;* \-#&quot; € &quot;;@\ "/>
-  </numFmts>
-  <fonts count="46">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="13">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color indexed="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="8"/>
-      <name val="ARIAL"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="8"/>
-      <name val="ARIAL"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="9"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Liberation Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="WenQuanYi Zen Hei"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Liberation Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Lohit Hindi"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Lohit Hindi"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Arial1"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="9"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="WenQuanYi Zen Hei"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="63"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="63"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="8.8000000000000007"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Liberation Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="9"/>
+      <color rgb="00000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="9"/>
+      <color rgb="00000000"/>
+      <name val="ARIAL"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="9"/>
+      <color rgb="00000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="9"/>
+      <color rgb="00000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="9"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="8"/>
-      <color indexed="8"/>
+      <color rgb="00000000"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="20"/>
       <color rgb="FFC00000"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -455,36 +339,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor indexed="26"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-        <bgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="26"/>
+        <fgColor rgb="00FFFFFF"/>
+        <bgColor rgb="00FFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="00FFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000AE00"/>
+        <bgColor rgb="00339966"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -494,90 +372,179 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color rgb="00000000"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color rgb="00000000"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color rgb="00000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color rgb="00000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00333333"/>
+      </right>
+      <top style="thin">
+        <color rgb="00333333"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00333333"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00333333"/>
+      </left>
+      <right style="thin">
+        <color rgb="00333333"/>
+      </right>
+      <top style="thin">
+        <color rgb="00333333"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00333333"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color rgb="00333333"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="8"/>
+        <color rgb="00333333"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color rgb="00333333"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00333333"/>
+      </right>
+      <top style="thin">
+        <color rgb="00333333"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color rgb="00333333"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color rgb="00333333"/>
+      </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color rgb="00333333"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color rgb="00000000"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color rgb="00000000"/>
       </right>
       <top/>
       <bottom/>
@@ -585,916 +552,527 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
+        <color rgb="00000000"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="00000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="00000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="63"/>
-      </left>
-      <right style="thin">
-        <color indexed="63"/>
-      </right>
-      <top style="thin">
-        <color indexed="63"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="63"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="63"/>
-      </right>
-      <top style="thin">
-        <color indexed="63"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="63"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="63"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="63"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="63"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="63"/>
-      </right>
-      <top style="thin">
-        <color indexed="63"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="63"/>
-      </left>
-      <right style="thin">
-        <color indexed="63"/>
-      </right>
-      <top style="thin">
-        <color indexed="63"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="104">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="15" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="15" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="15" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="157">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="60" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="60" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="60" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="60" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="1" xfId="60" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="60" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="60" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="60" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="60" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="60" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="60" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="8" xfId="60" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="2" xfId="60" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="93" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="60" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="95" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="95" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="95" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="95" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="89" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="14" fillId="0" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="3" fillId="3" borderId="4" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="3" fillId="3" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="14" fillId="0" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="3" fillId="0" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="14" fillId="3" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="1" fillId="4" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="3" fillId="0" borderId="5" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="3" fillId="0" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="5" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="5" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="5" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="5" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="5" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="14" fillId="3" borderId="4" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="14" fillId="4" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="3" fillId="0" borderId="7" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="3" fillId="2" borderId="7" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="49" fillId="2" borderId="7" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="3" fillId="0" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="3" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="3" fillId="0" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="49" fillId="0" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="3" fillId="0" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="4" fillId="0" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="3" fillId="0" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="3" fillId="0" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="3" fillId="0" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="3" fillId="0" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="1" fillId="0" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="14" fillId="0" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="8" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="1" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="9" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="5" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="5" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="16" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="14" fillId="4" borderId="5" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="14" fillId="4" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="10" numFmtId="0" fillId="5" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="14" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="1" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="14" fillId="2" borderId="7" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="14" fillId="2" borderId="7" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection locked="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="11" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="12" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="11" numFmtId="0" fillId="0" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="11" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="104">
-    <cellStyle name="Estilo 1" xfId="1"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in " xfId="2"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in " xfId="3"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in " xfId="4"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="5"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="6"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="7"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2 2" xfId="8"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2 2 2 2" xfId="9"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 3" xfId="10"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="11"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="12"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="13"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="14"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="15"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="16"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="17"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="18"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="19"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Explanatory Text" xfId="20"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Normal" xfId="21"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="22"/>
-    <cellStyle name="Excel Built-in Excel Built-in Explanatory Text" xfId="23"/>
-    <cellStyle name="Excel Built-in Excel Built-in Normal" xfId="24"/>
-    <cellStyle name="Excel Built-in Excel Built-in TableStyleLight1" xfId="25"/>
-    <cellStyle name="Excel Built-in Normal" xfId="26"/>
-    <cellStyle name="Excel Built-in Normal 2" xfId="27"/>
-    <cellStyle name="Excel Built-in Normal 3" xfId="28"/>
-    <cellStyle name="Excel Built-in Normal 4" xfId="29"/>
-    <cellStyle name="Excel Built-in Normal 9 7" xfId="30"/>
-    <cellStyle name="Excel Built-in TableStyleLight1" xfId="31"/>
-    <cellStyle name="Hipervínculo 2" xfId="32"/>
-    <cellStyle name="Hipervínculo 2 2" xfId="33"/>
-    <cellStyle name="Millares 2" xfId="34"/>
-    <cellStyle name="Millares 3" xfId="35"/>
-    <cellStyle name="Millares 4" xfId="36"/>
-    <cellStyle name="Moneda 2" xfId="37"/>
-    <cellStyle name="Moneda 2 2" xfId="38"/>
-    <cellStyle name="Moneda 3" xfId="39"/>
-    <cellStyle name="Moneda 4" xfId="40"/>
-    <cellStyle name="Moneda 6" xfId="41"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 110" xfId="42"/>
-    <cellStyle name="Normal 110 2" xfId="43"/>
-    <cellStyle name="Normal 13" xfId="44"/>
-    <cellStyle name="Normal 13 2" xfId="45"/>
-    <cellStyle name="Normal 13 3" xfId="46"/>
-    <cellStyle name="Normal 2" xfId="47"/>
-    <cellStyle name="Normal 2 2" xfId="48"/>
-    <cellStyle name="Normal 2 2 2" xfId="49"/>
-    <cellStyle name="Normal 2 2 2 2" xfId="50"/>
-    <cellStyle name="Normal 2 3" xfId="51"/>
-    <cellStyle name="Normal 2 3 2" xfId="52"/>
-    <cellStyle name="Normal 2 4" xfId="53"/>
-    <cellStyle name="Normal 2 4 2" xfId="54"/>
-    <cellStyle name="Normal 2 4 2 2" xfId="55"/>
-    <cellStyle name="Normal 2 4 3" xfId="56"/>
-    <cellStyle name="Normal 2 4 4" xfId="57"/>
-    <cellStyle name="Normal 2 5" xfId="58"/>
-    <cellStyle name="Normal 2 5 2" xfId="59"/>
-    <cellStyle name="Normal 3" xfId="60"/>
-    <cellStyle name="Normal 3 2" xfId="61"/>
-    <cellStyle name="Normal 3 2 2" xfId="62"/>
-    <cellStyle name="Normal 3 2 2 2" xfId="63"/>
-    <cellStyle name="Normal 3 2 2 2 2" xfId="64"/>
-    <cellStyle name="Normal 3 2 3" xfId="65"/>
-    <cellStyle name="Normal 3 2 4" xfId="66"/>
-    <cellStyle name="Normal 3 3" xfId="67"/>
-    <cellStyle name="Normal 3 3 2" xfId="68"/>
-    <cellStyle name="Normal 4" xfId="69"/>
-    <cellStyle name="Normal 4 2" xfId="70"/>
-    <cellStyle name="Normal 4 2 2" xfId="71"/>
-    <cellStyle name="Normal 4 3" xfId="72"/>
-    <cellStyle name="Normal 4 4" xfId="73"/>
-    <cellStyle name="Normal 5" xfId="74"/>
-    <cellStyle name="Normal 5 2" xfId="75"/>
-    <cellStyle name="Normal 5 2 2" xfId="76"/>
-    <cellStyle name="Normal 5 2 3" xfId="77"/>
-    <cellStyle name="Normal 5 3" xfId="78"/>
-    <cellStyle name="Normal 5 4" xfId="79"/>
-    <cellStyle name="Normal 6" xfId="80"/>
-    <cellStyle name="Normal 6 2" xfId="81"/>
-    <cellStyle name="Normal 6 3" xfId="82"/>
-    <cellStyle name="Normal 7" xfId="83"/>
-    <cellStyle name="Normal 7 2" xfId="84"/>
-    <cellStyle name="Normal 7 3" xfId="85"/>
-    <cellStyle name="Normal 9 7" xfId="86"/>
-    <cellStyle name="Normal 9 7 2" xfId="87"/>
-    <cellStyle name="Porcentaje 2" xfId="88"/>
-    <cellStyle name="Porcentaje 2 2" xfId="89"/>
-    <cellStyle name="Porcentaje 2 3" xfId="90"/>
-    <cellStyle name="Porcentaje 3" xfId="91"/>
-    <cellStyle name="Porcentaje 3 2" xfId="92"/>
-    <cellStyle name="Porcentaje 4" xfId="93"/>
-    <cellStyle name="Porcentual 2" xfId="94"/>
-    <cellStyle name="TableStyleLight1" xfId="95"/>
-    <cellStyle name="TableStyleLight1 2" xfId="96"/>
-    <cellStyle name="TableStyleLight1 2 2" xfId="97"/>
-    <cellStyle name="TableStyleLight1 2 3" xfId="98"/>
-    <cellStyle name="TableStyleLight1 3" xfId="99"/>
-    <cellStyle name="TableStyleLight1 3 2" xfId="100"/>
-    <cellStyle name="TableStyleLight1 4" xfId="101"/>
-    <cellStyle name="TableStyleLight1 4 2" xfId="102"/>
-    <cellStyle name="TableStyleLight1 5" xfId="103"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="0000AE00"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="001A1A1A"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00212121"/>
-      <rgbColor rgb="003A3935"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -1515,39 +1093,24 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1572" name="1 Imagen" descr="Recorte de pantalla">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000024060000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="1" name="1 Imagen" descr="Recorte de pantalla"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="27441525"/>
+      <xdr:spPr>
+        <a:xfrm rot="0">
           <a:ext cx="9525" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1567,39 +1130,24 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1573" name="2 Imagen" descr="Recorte de pantalla">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000025060000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="2 Imagen" descr="Recorte de pantalla"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="27441525"/>
+      <xdr:spPr>
+        <a:xfrm rot="0">
           <a:ext cx="9525" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1619,39 +1167,24 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1574" name="1 Imagen" descr="Recorte de pantalla">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000026060000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="1 Imagen" descr="Recorte de pantalla"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="27441525"/>
+      <xdr:spPr>
+        <a:xfrm rot="0">
           <a:ext cx="9525" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1671,39 +1204,24 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1575" name="2 Imagen" descr="Recorte de pantalla">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000027060000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="4" name="2 Imagen" descr="Recorte de pantalla"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="27441525"/>
+      <xdr:spPr>
+        <a:xfrm rot="0">
           <a:ext cx="9525" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1712,7 +1230,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1989,314 +1507,385 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1" cy="1"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst/>
-        </a:custGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-      </a:spPr>
-      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
-      <a:lstStyle/>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1" cy="1"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst/>
-        </a:custGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-      </a:spPr>
-      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
-      <a:lstStyle/>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:AJ63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr customHeight="true" defaultRowHeight="12.75" defaultColWidth="11.5703125" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="15" customWidth="1"/>
-    <col min="5" max="6" width="8.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
-    <col min="12" max="12" width="18" customWidth="1"/>
-    <col min="13" max="13" width="35.42578125" customWidth="1"/>
-    <col min="14" max="14" width="23.42578125" customWidth="1"/>
-    <col min="15" max="15" width="25.85546875" customWidth="1"/>
-    <col min="16" max="16" width="22.28515625" customWidth="1"/>
-    <col min="17" max="17" width="26" customWidth="1"/>
-    <col min="18" max="18" width="26.7109375" customWidth="1"/>
-    <col min="19" max="19" width="12.5703125" customWidth="1"/>
-    <col min="20" max="20" width="17.42578125" customWidth="1"/>
-    <col min="21" max="21" width="11.28515625" customWidth="1"/>
-    <col min="22" max="22" width="14.5703125" customWidth="1"/>
-    <col min="23" max="23" width="18.28515625" customWidth="1"/>
-    <col min="24" max="24" width="25.5703125" customWidth="1"/>
-    <col min="25" max="25" width="20.140625" customWidth="1"/>
-    <col min="26" max="26" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.7109375" customWidth="1"/>
-    <col min="28" max="28" width="10.42578125" customWidth="1"/>
-    <col min="29" max="29" width="16.7109375" customWidth="1"/>
-    <col min="30" max="30" width="19.28515625" customWidth="1"/>
-    <col min="31" max="31" width="18.5703125" customWidth="1"/>
-    <col min="32" max="32" width="17.28515625" customWidth="1"/>
-    <col min="33" max="33" width="60" customWidth="1"/>
-    <col min="34" max="34" width="24.5703125" style="16" customWidth="1"/>
-    <col min="35" max="35" width="19.85546875" style="16" customWidth="1"/>
-    <col min="36" max="36" width="23.28515625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="true" style="0"/>
+    <col min="2" max="2" width="13.42578125" customWidth="true" style="0"/>
+    <col min="3" max="3" width="15.5703125" customWidth="true" style="0"/>
+    <col min="4" max="4" width="14.42578125" customWidth="true" style="15"/>
+    <col min="5" max="5" width="8.5703125" customWidth="true" style="0"/>
+    <col min="6" max="6" width="8.5703125" customWidth="true" style="0"/>
+    <col min="7" max="7" width="10.28515625" customWidth="true" style="0"/>
+    <col min="8" max="8" width="8.5703125" customWidth="true" style="0"/>
+    <col min="9" max="9" width="18" customWidth="true" style="0"/>
+    <col min="10" max="10" width="17.140625" customWidth="true" style="0"/>
+    <col min="11" max="11" width="20.7109375" customWidth="true" style="0"/>
+    <col min="12" max="12" width="18" customWidth="true" style="0"/>
+    <col min="13" max="13" width="35.42578125" customWidth="true" style="0"/>
+    <col min="14" max="14" width="23.42578125" customWidth="true" style="0"/>
+    <col min="15" max="15" width="25.85546875" customWidth="true" style="0"/>
+    <col min="16" max="16" width="22.28515625" customWidth="true" style="0"/>
+    <col min="17" max="17" width="26" customWidth="true" style="0"/>
+    <col min="18" max="18" width="26.7109375" customWidth="true" style="0"/>
+    <col min="19" max="19" width="12.5703125" customWidth="true" style="0"/>
+    <col min="20" max="20" width="17.42578125" customWidth="true" style="0"/>
+    <col min="21" max="21" width="11.28515625" customWidth="true" style="0"/>
+    <col min="22" max="22" width="14.5703125" customWidth="true" style="0"/>
+    <col min="23" max="23" width="18.28515625" customWidth="true" style="0"/>
+    <col min="24" max="24" width="25.5703125" customWidth="true" style="0"/>
+    <col min="25" max="25" width="20.140625" customWidth="true" style="0"/>
+    <col min="26" max="26" width="12.85546875" customWidth="true" style="0"/>
+    <col min="27" max="27" width="9.7109375" customWidth="true" style="0"/>
+    <col min="28" max="28" width="10.42578125" customWidth="true" style="0"/>
+    <col min="29" max="29" width="16.7109375" customWidth="true" style="0"/>
+    <col min="30" max="30" width="19.28515625" customWidth="true" style="0"/>
+    <col min="31" max="31" width="18.5703125" customWidth="true" style="0"/>
+    <col min="32" max="32" width="17.28515625" customWidth="true" style="0"/>
+    <col min="33" max="33" width="60" customWidth="true" style="0"/>
+    <col min="34" max="34" width="24.5703125" customWidth="true" style="16"/>
+    <col min="35" max="35" width="19.85546875" customWidth="true" style="16"/>
+    <col min="36" max="36" width="23.28515625" customWidth="true" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="26.25" customHeight="1">
+    <row r="1" spans="1:36" customHeight="1" ht="26.25">
       <c r="A1" s="138" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="155" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="155"/>
+      <c r="B1" s="153" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="153"/>
       <c r="D1" s="140"/>
-      <c r="E1" s="156"/>
-      <c r="F1" s="156"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
       <c r="G1" s="140"/>
       <c r="H1" s="151"/>
-      <c r="I1" s="154" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="154"/>
-      <c r="K1" s="154"/>
-      <c r="L1" s="154"/>
-      <c r="M1" s="154"/>
-      <c r="N1" s="154"/>
-    </row>
-    <row r="2" spans="1:36" ht="12.75" customHeight="1">
+      <c r="I1" s="152" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="152"/>
+      <c r="K1" s="152"/>
+      <c r="L1" s="152"/>
+      <c r="M1" s="152"/>
+      <c r="N1" s="152"/>
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1"/>
+      <c r="R1"/>
+      <c r="S1"/>
+      <c r="T1"/>
+      <c r="U1"/>
+      <c r="V1"/>
+      <c r="W1"/>
+      <c r="X1"/>
+      <c r="Y1"/>
+      <c r="Z1"/>
+      <c r="AA1"/>
+      <c r="AB1"/>
+      <c r="AC1"/>
+      <c r="AD1"/>
+      <c r="AE1"/>
+      <c r="AF1"/>
+      <c r="AG1"/>
+      <c r="AH1"/>
+      <c r="AI1"/>
+      <c r="AJ1"/>
+    </row>
+    <row r="2" spans="1:36" customHeight="1" ht="12.75">
       <c r="A2" s="139">
         <v>0</v>
       </c>
-      <c r="B2" s="152" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="152"/>
+      <c r="B2" s="155" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="155"/>
       <c r="D2" s="141"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
       <c r="G2" s="141"/>
-      <c r="H2" s="153"/>
-      <c r="I2" s="153"/>
-    </row>
-    <row r="3" spans="1:36" ht="12.75" customHeight="1">
+      <c r="H2" s="156"/>
+      <c r="I2" s="156"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+      <c r="AB2"/>
+      <c r="AC2"/>
+      <c r="AD2"/>
+      <c r="AE2"/>
+      <c r="AF2"/>
+      <c r="AG2"/>
+      <c r="AH2"/>
+      <c r="AI2"/>
+      <c r="AJ2"/>
+    </row>
+    <row r="3" spans="1:36" customHeight="1" ht="12.75">
       <c r="A3" s="139">
         <v>1</v>
       </c>
-      <c r="B3" s="152" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="152"/>
+      <c r="B3" s="155" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="155"/>
       <c r="D3" s="141"/>
-      <c r="E3" s="153"/>
-      <c r="F3" s="153"/>
+      <c r="E3" s="156"/>
+      <c r="F3" s="156"/>
       <c r="G3" s="141"/>
-      <c r="H3" s="153"/>
-      <c r="I3" s="153"/>
-    </row>
-    <row r="4" spans="1:36" ht="12.75" customHeight="1">
+      <c r="H3" s="156"/>
+      <c r="I3" s="156"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+      <c r="Z3"/>
+      <c r="AA3"/>
+      <c r="AB3"/>
+      <c r="AC3"/>
+      <c r="AD3"/>
+      <c r="AE3"/>
+      <c r="AF3"/>
+      <c r="AG3"/>
+      <c r="AH3"/>
+      <c r="AI3"/>
+      <c r="AJ3"/>
+    </row>
+    <row r="4" spans="1:36" customHeight="1" ht="12.75">
       <c r="A4" s="139">
         <v>2</v>
       </c>
-      <c r="B4" s="152" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="152"/>
+      <c r="B4" s="155" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="155"/>
       <c r="D4" s="141"/>
-      <c r="E4" s="153"/>
-      <c r="F4" s="153"/>
+      <c r="E4" s="156"/>
+      <c r="F4" s="156"/>
       <c r="G4" s="141"/>
-      <c r="H4" s="153"/>
-      <c r="I4" s="153"/>
-    </row>
-    <row r="5" spans="1:36" ht="12.75" customHeight="1">
+      <c r="H4" s="156"/>
+      <c r="I4" s="156"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="Y4"/>
+      <c r="Z4"/>
+      <c r="AA4"/>
+      <c r="AB4"/>
+      <c r="AC4"/>
+      <c r="AD4"/>
+      <c r="AE4"/>
+      <c r="AF4"/>
+      <c r="AG4"/>
+      <c r="AH4"/>
+      <c r="AI4"/>
+      <c r="AJ4"/>
+    </row>
+    <row r="5" spans="1:36" customHeight="1" ht="12.75">
       <c r="A5" s="139">
         <v>3</v>
       </c>
-      <c r="B5" s="152" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="152"/>
+      <c r="B5" s="155" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="155"/>
       <c r="D5" s="141"/>
-      <c r="E5" s="153"/>
-      <c r="F5" s="153"/>
+      <c r="E5" s="156"/>
+      <c r="F5" s="156"/>
       <c r="G5" s="141"/>
-      <c r="H5" s="153"/>
-      <c r="I5" s="153"/>
-    </row>
-    <row r="6" spans="1:36" ht="64.5" customHeight="1">
+      <c r="H5" s="156"/>
+      <c r="I5" s="156"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+      <c r="Y5"/>
+      <c r="Z5"/>
+      <c r="AA5"/>
+      <c r="AB5"/>
+      <c r="AC5"/>
+      <c r="AD5"/>
+      <c r="AE5"/>
+      <c r="AF5"/>
+      <c r="AG5"/>
+      <c r="AH5"/>
+      <c r="AI5"/>
+      <c r="AJ5"/>
+    </row>
+    <row r="6" spans="1:36" customHeight="1" ht="64.5">
       <c r="A6" s="53" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="125" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C6" s="125" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D6" s="126" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E6" s="126" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F6" s="126" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G6" s="126" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H6" s="126" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I6" s="126" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="J6" s="54" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="K6" s="54" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="L6" s="54" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="M6" s="137" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q6" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="R6" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="S6" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="T6" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="U6" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="V6" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="W6" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="X6" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y6" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z6" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA6" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB6" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC6" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD6" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE6" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="N6" s="54" t="s">
-        <v>12</v>
-      </c>
-      <c r="O6" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="P6" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q6" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="R6" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="S6" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="T6" s="54" t="s">
-        <v>18</v>
-      </c>
-      <c r="U6" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="V6" s="54" t="s">
-        <v>20</v>
-      </c>
-      <c r="W6" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="X6" s="54" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y6" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z6" s="54" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA6" s="54" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB6" s="54" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC6" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD6" s="56" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE6" s="56" t="s">
-        <v>29</v>
-      </c>
       <c r="AF6" s="56" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="AG6" s="56" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="AH6" s="56" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="AI6" s="56" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="AJ6" s="57" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:36" s="8" customFormat="1" ht="34.9" customHeight="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" customHeight="1" ht="34.9" s="8" customFormat="1">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -2322,16 +1911,16 @@
         <v>4</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>43</v>
@@ -2360,45 +1949,103 @@
       <c r="AI7" s="4"/>
       <c r="AJ7" s="59"/>
     </row>
-    <row r="8" spans="1:36" s="7" customFormat="1" ht="34.9" customHeight="1">
-      <c r="A8" s="49"/>
-      <c r="B8" s="78"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="146"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="147"/>
+    <row r="8" spans="1:36" customHeight="1" ht="34.9" s="7" customFormat="1">
+      <c r="A8" s="49">
+        <v>1</v>
+      </c>
+      <c r="B8" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="146" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="66">
+        <v>24</v>
+      </c>
+      <c r="F8" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="4">
+        <v>2025</v>
+      </c>
+      <c r="H8" s="147">
+        <v>3</v>
+      </c>
       <c r="I8" s="147"/>
       <c r="J8" s="147"/>
       <c r="K8" s="147"/>
       <c r="L8" s="147"/>
-      <c r="M8" s="66"/>
+      <c r="M8" s="66" t="s">
+        <v>48</v>
+      </c>
       <c r="N8" s="147"/>
-      <c r="O8" s="147"/>
-      <c r="P8" s="147"/>
-      <c r="Q8" s="67"/>
-      <c r="R8" s="79"/>
-      <c r="S8" s="68"/>
-      <c r="T8" s="67"/>
-      <c r="U8" s="80"/>
-      <c r="V8" s="68"/>
-      <c r="W8" s="67"/>
-      <c r="X8" s="50"/>
-      <c r="Y8" s="147"/>
-      <c r="Z8" s="69"/>
+      <c r="O8" s="147" t="s">
+        <v>49</v>
+      </c>
+      <c r="P8" s="147" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q8" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="R8" s="79" t="s">
+        <v>51</v>
+      </c>
+      <c r="S8" s="68">
+        <v>3</v>
+      </c>
+      <c r="T8" s="67">
+        <v>6</v>
+      </c>
+      <c r="U8" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="V8" s="68">
+        <v>5</v>
+      </c>
+      <c r="W8" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="X8" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y8" s="147" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z8" s="69" t="s">
+        <v>56</v>
+      </c>
       <c r="AA8" s="66"/>
       <c r="AB8" s="66"/>
-      <c r="AC8" s="147"/>
-      <c r="AD8" s="66"/>
-      <c r="AE8" s="66"/>
-      <c r="AF8" s="70"/>
-      <c r="AG8" s="147"/>
-      <c r="AH8" s="71"/>
-      <c r="AI8" s="66"/>
-      <c r="AJ8" s="59"/>
-    </row>
-    <row r="9" spans="1:36" s="7" customFormat="1" ht="34.9" customHeight="1">
+      <c r="AC8" s="147" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD8" s="66" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE8" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF8" s="70">
+        <v>3</v>
+      </c>
+      <c r="AG8" s="147" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH8" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI8" s="66">
+        <v>40000000004</v>
+      </c>
+      <c r="AJ8" s="59" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" customHeight="1" ht="34.9" s="7" customFormat="1">
       <c r="A9" s="72"/>
       <c r="B9" s="78"/>
       <c r="C9" s="76"/>
@@ -2436,7 +2083,7 @@
       <c r="AI9" s="73"/>
       <c r="AJ9" s="59"/>
     </row>
-    <row r="10" spans="1:36" s="7" customFormat="1" ht="34.9" customHeight="1">
+    <row r="10" spans="1:36" customHeight="1" ht="34.9" s="7" customFormat="1">
       <c r="A10" s="2"/>
       <c r="B10" s="76"/>
       <c r="C10" s="76"/>
@@ -2474,7 +2121,7 @@
       <c r="AI10" s="18"/>
       <c r="AJ10" s="59"/>
     </row>
-    <row r="11" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="11" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A11" s="2"/>
       <c r="B11" s="76"/>
       <c r="C11" s="76"/>
@@ -2512,7 +2159,7 @@
       <c r="AI11" s="18"/>
       <c r="AJ11" s="59"/>
     </row>
-    <row r="12" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="12" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A12" s="2"/>
       <c r="B12" s="76"/>
       <c r="C12" s="76"/>
@@ -2550,7 +2197,7 @@
       <c r="AI12" s="18"/>
       <c r="AJ12" s="59"/>
     </row>
-    <row r="13" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="13" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A13" s="2"/>
       <c r="B13" s="24"/>
       <c r="C13" s="64"/>
@@ -2588,7 +2235,7 @@
       <c r="AI13" s="82"/>
       <c r="AJ13" s="59"/>
     </row>
-    <row r="14" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="14" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A14" s="87"/>
       <c r="B14" s="33"/>
       <c r="C14" s="88"/>
@@ -2626,7 +2273,7 @@
       <c r="AI14" s="93"/>
       <c r="AJ14" s="59"/>
     </row>
-    <row r="15" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="15" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A15" s="94"/>
       <c r="B15" s="24"/>
       <c r="C15" s="64"/>
@@ -2664,7 +2311,7 @@
       <c r="AI15" s="107"/>
       <c r="AJ15" s="59"/>
     </row>
-    <row r="16" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="16" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A16" s="94"/>
       <c r="B16" s="33"/>
       <c r="C16" s="88"/>
@@ -2702,7 +2349,7 @@
       <c r="AI16" s="107"/>
       <c r="AJ16" s="59"/>
     </row>
-    <row r="17" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="17" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A17" s="94"/>
       <c r="B17" s="24"/>
       <c r="C17" s="64"/>
@@ -2740,7 +2387,7 @@
       <c r="AI17" s="107"/>
       <c r="AJ17" s="59"/>
     </row>
-    <row r="18" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="18" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A18" s="94"/>
       <c r="B18" s="33"/>
       <c r="C18" s="88"/>
@@ -2778,7 +2425,7 @@
       <c r="AI18" s="107"/>
       <c r="AJ18" s="59"/>
     </row>
-    <row r="19" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="19" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A19" s="94"/>
       <c r="B19" s="24"/>
       <c r="C19" s="64"/>
@@ -2816,7 +2463,7 @@
       <c r="AI19" s="107"/>
       <c r="AJ19" s="59"/>
     </row>
-    <row r="20" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="20" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A20" s="94"/>
       <c r="B20" s="24"/>
       <c r="C20" s="88"/>
@@ -2854,7 +2501,7 @@
       <c r="AI20" s="107"/>
       <c r="AJ20" s="59"/>
     </row>
-    <row r="21" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="21" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A21" s="94"/>
       <c r="B21" s="33"/>
       <c r="C21" s="64"/>
@@ -2892,7 +2539,7 @@
       <c r="AI21" s="107"/>
       <c r="AJ21" s="59"/>
     </row>
-    <row r="22" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="22" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A22" s="94"/>
       <c r="B22" s="24"/>
       <c r="C22" s="88"/>
@@ -2930,7 +2577,7 @@
       <c r="AI22" s="102"/>
       <c r="AJ22" s="59"/>
     </row>
-    <row r="23" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="23" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A23" s="94"/>
       <c r="B23" s="33"/>
       <c r="C23" s="64"/>
@@ -2968,7 +2615,7 @@
       <c r="AI23" s="102"/>
       <c r="AJ23" s="59"/>
     </row>
-    <row r="24" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="24" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A24" s="94"/>
       <c r="B24" s="33"/>
       <c r="C24" s="88"/>
@@ -3006,7 +2653,7 @@
       <c r="AI24" s="102"/>
       <c r="AJ24" s="59"/>
     </row>
-    <row r="25" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="25" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A25" s="2"/>
       <c r="B25" s="24"/>
       <c r="C25" s="64"/>
@@ -3044,7 +2691,7 @@
       <c r="AI25" s="102"/>
       <c r="AJ25" s="59"/>
     </row>
-    <row r="26" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="26" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A26" s="2"/>
       <c r="B26" s="33"/>
       <c r="C26" s="88"/>
@@ -3082,7 +2729,7 @@
       <c r="AI26" s="102"/>
       <c r="AJ26" s="59"/>
     </row>
-    <row r="27" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="27" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A27" s="2"/>
       <c r="B27" s="24"/>
       <c r="C27" s="64"/>
@@ -3120,7 +2767,7 @@
       <c r="AI27" s="102"/>
       <c r="AJ27" s="59"/>
     </row>
-    <row r="28" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="28" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A28" s="2"/>
       <c r="B28" s="33"/>
       <c r="C28" s="88"/>
@@ -3158,7 +2805,7 @@
       <c r="AI28" s="102"/>
       <c r="AJ28" s="59"/>
     </row>
-    <row r="29" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="29" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A29" s="2"/>
       <c r="B29" s="33"/>
       <c r="C29" s="64"/>
@@ -3196,7 +2843,7 @@
       <c r="AI29" s="102"/>
       <c r="AJ29" s="59"/>
     </row>
-    <row r="30" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="30" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A30" s="2"/>
       <c r="B30" s="24"/>
       <c r="C30" s="88"/>
@@ -3234,7 +2881,7 @@
       <c r="AI30" s="102"/>
       <c r="AJ30" s="59"/>
     </row>
-    <row r="31" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="31" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A31" s="2"/>
       <c r="B31" s="33"/>
       <c r="C31" s="64"/>
@@ -3272,7 +2919,7 @@
       <c r="AI31" s="102"/>
       <c r="AJ31" s="59"/>
     </row>
-    <row r="32" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="32" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A32" s="2"/>
       <c r="B32" s="33"/>
       <c r="C32" s="88"/>
@@ -3310,7 +2957,7 @@
       <c r="AI32" s="102"/>
       <c r="AJ32" s="59"/>
     </row>
-    <row r="33" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="33" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A33" s="2"/>
       <c r="B33" s="33"/>
       <c r="C33" s="64"/>
@@ -3348,7 +2995,7 @@
       <c r="AI33" s="102"/>
       <c r="AJ33" s="59"/>
     </row>
-    <row r="34" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="34" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A34" s="2"/>
       <c r="B34" s="24"/>
       <c r="C34" s="88"/>
@@ -3386,7 +3033,7 @@
       <c r="AI34" s="102"/>
       <c r="AJ34" s="59"/>
     </row>
-    <row r="35" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="35" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A35" s="2"/>
       <c r="B35" s="24"/>
       <c r="C35" s="64"/>
@@ -3424,7 +3071,7 @@
       <c r="AI35" s="102"/>
       <c r="AJ35" s="59"/>
     </row>
-    <row r="36" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="36" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A36" s="2"/>
       <c r="B36" s="24"/>
       <c r="C36" s="88"/>
@@ -3462,7 +3109,7 @@
       <c r="AI36" s="102"/>
       <c r="AJ36" s="59"/>
     </row>
-    <row r="37" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="37" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A37" s="2"/>
       <c r="B37" s="24"/>
       <c r="C37" s="64"/>
@@ -3500,7 +3147,7 @@
       <c r="AI37" s="102"/>
       <c r="AJ37" s="59"/>
     </row>
-    <row r="38" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="38" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A38" s="2"/>
       <c r="B38" s="24"/>
       <c r="C38" s="88"/>
@@ -3538,7 +3185,7 @@
       <c r="AI38" s="102"/>
       <c r="AJ38" s="59"/>
     </row>
-    <row r="39" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="39" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A39" s="2"/>
       <c r="B39" s="24"/>
       <c r="C39" s="64"/>
@@ -3576,7 +3223,7 @@
       <c r="AI39" s="102"/>
       <c r="AJ39" s="59"/>
     </row>
-    <row r="40" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="40" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A40" s="2"/>
       <c r="B40" s="24"/>
       <c r="C40" s="88"/>
@@ -3614,7 +3261,7 @@
       <c r="AI40" s="107"/>
       <c r="AJ40" s="59"/>
     </row>
-    <row r="41" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="41" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A41" s="2"/>
       <c r="B41" s="24"/>
       <c r="C41" s="64"/>
@@ -3652,7 +3299,7 @@
       <c r="AI41" s="107"/>
       <c r="AJ41" s="59"/>
     </row>
-    <row r="42" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="42" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A42" s="2"/>
       <c r="B42" s="24"/>
       <c r="C42" s="88"/>
@@ -3690,7 +3337,7 @@
       <c r="AI42" s="107"/>
       <c r="AJ42" s="59"/>
     </row>
-    <row r="43" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="43" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A43" s="2"/>
       <c r="B43" s="24"/>
       <c r="C43" s="64"/>
@@ -3728,7 +3375,7 @@
       <c r="AI43" s="107"/>
       <c r="AJ43" s="59"/>
     </row>
-    <row r="44" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="44" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A44" s="2"/>
       <c r="B44" s="24"/>
       <c r="C44" s="88"/>
@@ -3766,7 +3413,7 @@
       <c r="AI44" s="107"/>
       <c r="AJ44" s="59"/>
     </row>
-    <row r="45" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="45" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A45" s="94"/>
       <c r="B45" s="76"/>
       <c r="C45" s="88"/>
@@ -3804,7 +3451,7 @@
       <c r="AI45" s="4"/>
       <c r="AJ45" s="59"/>
     </row>
-    <row r="46" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="46" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A46" s="48"/>
       <c r="B46" s="64"/>
       <c r="C46" s="64"/>
@@ -3842,7 +3489,7 @@
       <c r="AI46" s="66"/>
       <c r="AJ46" s="59"/>
     </row>
-    <row r="47" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="47" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A47" s="114"/>
       <c r="B47" s="76"/>
       <c r="C47" s="88"/>
@@ -3880,7 +3527,7 @@
       <c r="AI47" s="73"/>
       <c r="AJ47" s="59"/>
     </row>
-    <row r="48" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="48" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A48" s="94"/>
       <c r="B48" s="64"/>
       <c r="C48" s="64"/>
@@ -3918,7 +3565,7 @@
       <c r="AI48" s="73"/>
       <c r="AJ48" s="59"/>
     </row>
-    <row r="49" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="49" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A49" s="2"/>
       <c r="B49" s="64"/>
       <c r="C49" s="88"/>
@@ -3956,7 +3603,7 @@
       <c r="AI49" s="73"/>
       <c r="AJ49" s="59"/>
     </row>
-    <row r="50" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="50" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A50" s="2"/>
       <c r="B50" s="76"/>
       <c r="C50" s="64"/>
@@ -3994,7 +3641,7 @@
       <c r="AI50" s="18"/>
       <c r="AJ50" s="59"/>
     </row>
-    <row r="51" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="51" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A51" s="32"/>
       <c r="B51" s="64"/>
       <c r="C51" s="88"/>
@@ -4032,7 +3679,7 @@
       <c r="AI51" s="29"/>
       <c r="AJ51" s="59"/>
     </row>
-    <row r="52" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="52" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A52" s="32"/>
       <c r="B52" s="64"/>
       <c r="C52" s="64"/>
@@ -4070,7 +3717,7 @@
       <c r="AI52" s="29"/>
       <c r="AJ52" s="59"/>
     </row>
-    <row r="53" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="53" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A53" s="32"/>
       <c r="B53" s="64"/>
       <c r="C53" s="88"/>
@@ -4108,7 +3755,7 @@
       <c r="AI53" s="29"/>
       <c r="AJ53" s="59"/>
     </row>
-    <row r="54" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="54" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A54" s="32"/>
       <c r="B54" s="64"/>
       <c r="C54" s="64"/>
@@ -4146,7 +3793,7 @@
       <c r="AI54" s="29"/>
       <c r="AJ54" s="59"/>
     </row>
-    <row r="55" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="55" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A55" s="32"/>
       <c r="B55" s="64"/>
       <c r="C55" s="88"/>
@@ -4184,7 +3831,7 @@
       <c r="AI55" s="29"/>
       <c r="AJ55" s="59"/>
     </row>
-    <row r="56" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="56" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A56" s="32"/>
       <c r="B56" s="64"/>
       <c r="C56" s="64"/>
@@ -4222,7 +3869,7 @@
       <c r="AI56" s="29"/>
       <c r="AJ56" s="59"/>
     </row>
-    <row r="57" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="57" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A57" s="32"/>
       <c r="B57" s="64"/>
       <c r="C57" s="88"/>
@@ -4260,7 +3907,7 @@
       <c r="AI57" s="29"/>
       <c r="AJ57" s="59"/>
     </row>
-    <row r="58" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="58" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A58" s="32"/>
       <c r="B58" s="64"/>
       <c r="C58" s="64"/>
@@ -4298,7 +3945,7 @@
       <c r="AI58" s="29"/>
       <c r="AJ58" s="59"/>
     </row>
-    <row r="59" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="59" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A59" s="32"/>
       <c r="B59" s="64"/>
       <c r="C59" s="88"/>
@@ -4336,7 +3983,7 @@
       <c r="AI59" s="29"/>
       <c r="AJ59" s="59"/>
     </row>
-    <row r="60" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="60" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A60" s="32"/>
       <c r="B60" s="88"/>
       <c r="C60" s="88"/>
@@ -4374,7 +4021,7 @@
       <c r="AI60" s="29"/>
       <c r="AJ60" s="59"/>
     </row>
-    <row r="61" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="61" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A61" s="127"/>
       <c r="B61" s="30"/>
       <c r="C61" s="30"/>
@@ -4412,7 +4059,7 @@
       <c r="AI61" s="29"/>
       <c r="AJ61" s="59"/>
     </row>
-    <row r="62" spans="1:36" s="9" customFormat="1" ht="34.9" customHeight="1">
+    <row r="62" spans="1:36" customHeight="1" ht="34.9" s="9" customFormat="1">
       <c r="A62" s="128"/>
       <c r="B62" s="30"/>
       <c r="C62" s="30"/>
@@ -4450,14 +4097,12 @@
       <c r="AI62" s="12"/>
       <c r="AJ62" s="59"/>
     </row>
+    <row r="63" spans="1:36">
+      <c r="A63"/>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="15">
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
+  <mergeCells>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="B5:C5"/>
@@ -4468,13 +4113,24 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
   </mergeCells>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter alignWithMargins="0">
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.0527777777778" bottom="1.0527777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" r:id="rId1ps"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
   <drawing r:id="rId2"/>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>